<commit_message>
first version of human numbers dataset in csv format
</commit_message>
<xml_diff>
--- a/datasets/_pub_g/_ds_g__ont/_dimensions.xlsx
+++ b/datasets/_pub_g/_ds_g__ont/_dimensions.xlsx
@@ -31,9 +31,6 @@
     <t>Geos</t>
   </si>
   <si>
-    <t>planet</t>
-  </si>
-  <si>
     <t>subdim</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>gui_countries</t>
+  </si>
+  <si>
+    <t>global</t>
   </si>
 </sst>
 </file>
@@ -353,6 +353,45 @@
   <dxfs count="21">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -380,7 +419,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -398,7 +437,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -416,19 +455,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -447,32 +473,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -491,7 +491,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -504,25 +504,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="8"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -558,7 +545,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -576,7 +563,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -594,7 +581,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -612,6 +599,19 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -630,7 +630,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -648,7 +648,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -696,24 +696,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="_dimensions" displayName="_dimensions" ref="A1:S8" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <tableColumns count="19">
     <tableColumn id="1" name="concept" dataDxfId="18"/>
-    <tableColumn id="25" name="name" dataDxfId="5"/>
-    <tableColumn id="16" name="user" dataDxfId="3"/>
-    <tableColumn id="2" name="type" dataDxfId="4"/>
-    <tableColumn id="20" name="value_type" dataDxfId="0"/>
-    <tableColumn id="19" name="dimension" dataDxfId="17"/>
-    <tableColumn id="21" name="default_entities" dataDxfId="16"/>
-    <tableColumn id="10" name="parent_entitiy" dataDxfId="1"/>
-    <tableColumn id="5" name="name_short" dataDxfId="15"/>
-    <tableColumn id="14" name="name_long" dataDxfId="14"/>
-    <tableColumn id="15" name="plural" dataDxfId="13"/>
-    <tableColumn id="23" name="plural_short" dataDxfId="12"/>
-    <tableColumn id="24" name="plural_long" dataDxfId="11"/>
-    <tableColumn id="4" name="description" dataDxfId="10"/>
-    <tableColumn id="17" name="links" dataDxfId="9"/>
-    <tableColumn id="18" name="aliases" dataDxfId="8"/>
-    <tableColumn id="13" name="tags" dataDxfId="7"/>
-    <tableColumn id="3" name="color_schema" dataDxfId="6"/>
-    <tableColumn id="8" name="geo_shapes" dataDxfId="2"/>
+    <tableColumn id="25" name="name" dataDxfId="17"/>
+    <tableColumn id="16" name="user" dataDxfId="16"/>
+    <tableColumn id="2" name="type" dataDxfId="15"/>
+    <tableColumn id="20" name="value_type" dataDxfId="14"/>
+    <tableColumn id="19" name="dimension" dataDxfId="13"/>
+    <tableColumn id="21" name="default_entities" dataDxfId="12"/>
+    <tableColumn id="10" name="parent_entitiy" dataDxfId="11"/>
+    <tableColumn id="5" name="name_short" dataDxfId="10"/>
+    <tableColumn id="14" name="name_long" dataDxfId="9"/>
+    <tableColumn id="15" name="plural" dataDxfId="8"/>
+    <tableColumn id="23" name="plural_short" dataDxfId="7"/>
+    <tableColumn id="24" name="plural_long" dataDxfId="6"/>
+    <tableColumn id="4" name="description" dataDxfId="5"/>
+    <tableColumn id="17" name="links" dataDxfId="4"/>
+    <tableColumn id="18" name="aliases" dataDxfId="3"/>
+    <tableColumn id="13" name="tags" dataDxfId="2"/>
+    <tableColumn id="3" name="color_schema" dataDxfId="1"/>
+    <tableColumn id="8" name="geo_shapes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1009,10 +1009,10 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,58 +1045,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1113,36 +1113,36 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="5"/>
@@ -1150,154 +1150,154 @@
     </row>
     <row r="3" spans="1:19" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="O3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
     </row>
     <row r="4" spans="1:19" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="M4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="P4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
     </row>
     <row r="5" spans="1:19" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="8">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="P5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="5"/>
@@ -1305,104 +1305,104 @@
     </row>
     <row r="6" spans="1:19" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="8">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="P6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
     </row>
     <row r="7" spans="1:19" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="5"/>
@@ -1410,51 +1410,51 @@
     </row>
     <row r="8" spans="1:19" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="9">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="L8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="5"/>
       <c r="Q8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>

</xml_diff>